<commit_message>
paper read and summary
</commit_message>
<xml_diff>
--- a/文件系统/文件系统相关的论文-时间排序.xlsx
+++ b/文件系统/文件系统相关的论文-时间排序.xlsx
@@ -141,43 +141,43 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x0002_actional memory. In 20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>9 49th Annual IEEE/IFIP I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ter_x0002_national Conference on Dependable Systems and Net_x0002_works (DSN), pages 151–163, 2019.</t>
+      <t>x005f_x0002_actional memory.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>In 2019 49th Annual IEEE/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>FIP Inter_x0002_national Conference on Dependable Systems and Net_x0002_works (DSN), pages 151–163, 2019.</t>
     </r>
   </si>
   <si>
@@ -207,7 +207,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_ings of the 2017 USENIX Conference on Usenix Annual
+      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_ings of the 2017 USENIX Conference on Usenix Annual
 Technical Conference, USENIX ATC ’17, page 719–731.
 USENIX Association, 2017.</t>
     </r>
@@ -248,25 +248,25 @@
         <charset val="134"/>
       </rPr>
       <t>x005f_x0002_ence on Usenix Annual Technical Conference, USENIX
-ATC ’17, pages 703</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>–</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>717, USA, 2017. USENIX Associ_x0002_ation.</t>
+ATC ’17, pag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>s 703–717, USA, 2017. USENIX Associ_x0002_ation.</t>
     </r>
   </si>
   <si>
@@ -296,7 +296,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_ries. In 14th USENIX Conference on File and Storage
+      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_ries. In 14th USENIX Conference on File and Storage
 Technologies (FAST 16), pages 323–338, 2016.</t>
     </r>
   </si>
@@ -332,25 +332,25 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x0002_Won Lee, and Young I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Eom. Lightweight Application_x0002_Level crash consistency on transactional flash storage. In
+      <t>x005f_x0002_Won Lee, and Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ung Ik Eom. Lightweight Application_x0002_Level crash consistency on transactional flash storage. In
 2015 USENIX Annual Technical Conference (USENIX
 ATC 15), pages 221–234, Santa Clara, CA, July 2015.
 USENIX Association.</t>
@@ -382,25 +382,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x0002_Won Lee, and Young I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Eom. Lightweight Applicati</t>
+      <t>x005f_x0002_Won Lee, and Y</t>
     </r>
     <r>
       <rPr>
@@ -418,7 +400,25 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>n_x0002_Level Crash Consistency on Transactional Flash Stor_x0002_age. In Proc. of USENIX Annual Technical Conference
+      <t>ung Ik Eom. Lightweight App</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ication_x0002_Level Crash Consistency on Transactional Flash Stor_x0002_age. In Proc. of USENIX Annual Technical Conference
 (ATC), 2015.</t>
     </r>
   </si>
@@ -455,25 +455,25 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_murthy, Philip L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ntz, Dheeraj Reddy, Rajesh Sankaran,
+      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_x005f_x005f_x0002_murthy, Philip Lantz, Dheeraj Reddy, Rajesh Sankaran,
 and Jeff Jackson. System software for persistent mem_x0002_ory. In Proceedings of the Ninth European Conference
 on Computer Systems, pages 1–15, 2014</t>
     </r>
@@ -504,26 +504,26 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_vam, Venkatanathan Varadarajan, Prashant Saxena, and
-Michael M. Swift. Aeri</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>: Flexible file-system interfaces
+      <t>x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_vam, Venkatanathan Varadarajan, Prashan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Saxena, and
+Michael M. Swift. Aerie: Flexible file-system interfaces
 to storage-class memory. In Proceedings of the Ninth Eu_x0002_ropean Conference on Computer Systems, EuroSys ’14,pages 14:1–14:14, New York, NY, USA, 2014. ACM.</t>
     </r>
   </si>
@@ -554,7 +554,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x005f_</t>
+      <t>x005f_x005f_</t>
     </r>
     <r>
       <rPr>
@@ -572,7 +572,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>005f_x005f_x005f_x005f_x005f_x0002_rick Coetzee. Better i/o through byte-addressable, per_x0002_sistent memory. In Proceedings of the ACM SIGOPS
+      <t>005f_x005f_x005f_x005f_x005f_x005f_x005f_x005f_x0002_rick Coetzee. Better i/o through byte-addressable, per_x0002_sistent memory. In Proceedings of the ACM SIGOPS
 22nd symposium on Operating systems principles, pages
 133–146, 2009.</t>
     </r>
@@ -767,7 +767,25 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>x005f_x005f_x0002_dona. SI</t>
+      <t>x005f_x005f_x005f_x0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5f_x0002_dona. SI</t>
     </r>
     <r>
       <rPr>
@@ -785,25 +803,7 @@
         <rFont val="Microsoft YaHei"/>
         <charset val="134"/>
       </rPr>
-      <t>K: Preventing Lat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ncy Spikes in Log_x0002_Structured Merge Key-Value Stores. In Proc. of USENIX
+      <t>K: Preventing Latency Spikes in Log_x0002_Structured Merge Key-Value Stores. In Proc. of USENIX
 Annual Technical Conference (ATC), 2019.</t>
     </r>
   </si>
@@ -2068,7 +2068,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>